<commit_message>
Added analysis and synthesisfiles
</commit_message>
<xml_diff>
--- a/Synthesis/Trial synthesis 2 (tongali)/Modal Distribution Program Parameter Changes.xlsx
+++ b/Synthesis/Trial synthesis 2 (tongali)/Modal Distribution Program Parameter Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianbagaforo/Desktop/ECE198/Synthesis/Trial synthesis 2 (tongali)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7BE7DA-C95A-1A44-89FB-6D80252E478E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B602CE6-687A-BC42-A1E3-31D56908DC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11380" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="158" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>File number</t>
   </si>
@@ -56,13 +56,85 @@
   </si>
   <si>
     <t>Stereo file number</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>9b</t>
+  </si>
+  <si>
+    <t>10a</t>
+  </si>
+  <si>
+    <t>11b</t>
+  </si>
+  <si>
+    <t>12a</t>
+  </si>
+  <si>
+    <t>Based on recording 158 of the tongali provided by UP DSP. Audio normalized using Audacity</t>
+  </si>
+  <si>
+    <t>Partial number (60 dB)</t>
+  </si>
+  <si>
+    <t>Partial number (80 dB)</t>
+  </si>
+  <si>
+    <t>Partial number (100 dB)</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>denoised, trimmed, and normalized.</t>
+  </si>
+  <si>
+    <t>REPEAT BITCH</t>
+  </si>
+  <si>
+    <t>IYAK KA NA LANG</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>Partial number (90 dB)</t>
+  </si>
+  <si>
+    <t>Partial number (70 dB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -72,10 +144,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,14 +174,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,382 +420,1732 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C59BEEC-493C-794E-B0E6-018788CAA36A}">
-  <dimension ref="A2:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G26"/>
+    <sheetView tabSelected="1" topLeftCell="H23" zoomScale="91" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>8192</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>31.25</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>15.99</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1742.52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1780.18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>2342.6999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2153.61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1732.38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>6</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2265.62</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
         <v>7</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2037.39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1957.55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
         <v>19</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>9</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1897.55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
         <v>20</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>10</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1706.17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
         <v>23</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>11</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1647.26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14">
+    <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
         <v>24</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="3">
         <v>1772.77</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>13</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>206</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1756.26</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>134</v>
+      </c>
+      <c r="N15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>14</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>255</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1.97</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1780.18</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <v>58</v>
+      </c>
+      <c r="L16">
+        <v>107</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B17">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>15</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>283</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1.75</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>2342.6999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="H17">
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <v>41</v>
+      </c>
+      <c r="L17">
+        <v>76</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B18">
         <v>8</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>16</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>326</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1.52</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>2153.61</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="H18">
+        <v>43</v>
+      </c>
+      <c r="J18">
+        <v>44</v>
+      </c>
+      <c r="L18">
+        <v>245</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B19">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>17</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>373</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>1.34</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>1732.38</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="H19">
+        <v>128</v>
+      </c>
+      <c r="J19">
+        <v>128</v>
+      </c>
+      <c r="L19">
+        <v>135</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B20">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>18</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>430</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>2265.62</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="H20">
+        <v>106</v>
+      </c>
+      <c r="J20">
+        <v>106</v>
+      </c>
+      <c r="L20">
+        <v>128</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B21">
         <v>14</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>19</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>515</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>0.98</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>2037.39</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="H21">
+        <v>82</v>
+      </c>
+      <c r="J21">
+        <v>82</v>
+      </c>
+      <c r="L21">
+        <v>56</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B22">
         <v>16</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>580</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.88</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>1957.55</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="H22">
+        <v>106</v>
+      </c>
+      <c r="J22">
+        <v>106</v>
+      </c>
+      <c r="L22">
+        <v>55</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B23">
         <v>19</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>21</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>660</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>0.75</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>1897.55</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="H23">
+        <v>166</v>
+      </c>
+      <c r="J23">
+        <v>166</v>
+      </c>
+      <c r="L23">
+        <v>253</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B24">
         <v>20</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>22</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>768</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>0.66</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>1706.17</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>23</v>
-      </c>
+      <c r="H24">
+        <v>214</v>
+      </c>
+      <c r="J24">
+        <v>214</v>
+      </c>
+      <c r="L24">
+        <v>42</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B25">
         <v>23</v>
       </c>
-      <c r="D25">
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="E25">
         <v>886</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>1647.26</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26">
+      <c r="H25">
+        <v>284</v>
+      </c>
+      <c r="J25">
+        <v>284</v>
+      </c>
+      <c r="L25">
+        <v>66</v>
+      </c>
+      <c r="N25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="O25" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="3">
         <v>24</v>
       </c>
-      <c r="D26">
+      <c r="C26" s="3">
+        <v>24</v>
+      </c>
+      <c r="E26" s="3">
         <v>919</v>
       </c>
-      <c r="E26">
+      <c r="F26" s="3">
         <v>0.52</v>
       </c>
-      <c r="F26">
+      <c r="G26" s="3">
         <v>1772.77</v>
+      </c>
+      <c r="H26" s="3">
+        <v>264</v>
+      </c>
+      <c r="J26" s="3">
+        <v>264</v>
+      </c>
+      <c r="L26" s="3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>211</v>
+      </c>
+      <c r="F27">
+        <v>2.38</v>
+      </c>
+      <c r="G27">
+        <v>1756.26</v>
+      </c>
+      <c r="H27">
+        <v>18</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
+      </c>
+      <c r="L27">
+        <v>124</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="E28">
+        <v>260</v>
+      </c>
+      <c r="F28">
+        <v>1.93</v>
+      </c>
+      <c r="G28">
+        <v>1780.18</v>
+      </c>
+      <c r="H28">
+        <v>72</v>
+      </c>
+      <c r="J28">
+        <v>72</v>
+      </c>
+      <c r="L28">
+        <v>116</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>288</v>
+      </c>
+      <c r="F29">
+        <v>1.75</v>
+      </c>
+      <c r="G29">
+        <v>2342.6999999999998</v>
+      </c>
+      <c r="H29">
+        <v>41</v>
+      </c>
+      <c r="J29">
+        <v>41</v>
+      </c>
+      <c r="L29">
+        <v>78</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O29" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>331</v>
+      </c>
+      <c r="F30">
+        <v>1.52</v>
+      </c>
+      <c r="G30">
+        <v>2153.61</v>
+      </c>
+      <c r="H30">
+        <v>43</v>
+      </c>
+      <c r="J30">
+        <v>43</v>
+      </c>
+      <c r="L30">
+        <v>249</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>378</v>
+      </c>
+      <c r="F31">
+        <v>1.34</v>
+      </c>
+      <c r="G31">
+        <v>1732.38</v>
+      </c>
+      <c r="H31">
+        <v>126</v>
+      </c>
+      <c r="J31">
+        <v>126</v>
+      </c>
+      <c r="L31">
+        <v>140</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O31" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>435</v>
+      </c>
+      <c r="F32">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G32">
+        <v>2565.62</v>
+      </c>
+      <c r="H32">
+        <v>109</v>
+      </c>
+      <c r="J32">
+        <v>109</v>
+      </c>
+      <c r="L32">
+        <v>137</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>520</v>
+      </c>
+      <c r="F33">
+        <v>0.98</v>
+      </c>
+      <c r="G33">
+        <v>2037.39</v>
+      </c>
+      <c r="H33">
+        <v>77</v>
+      </c>
+      <c r="J33">
+        <v>77</v>
+      </c>
+      <c r="L33">
+        <v>53</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>585</v>
+      </c>
+      <c r="F34">
+        <v>0.84</v>
+      </c>
+      <c r="G34">
+        <v>1957.55</v>
+      </c>
+      <c r="H34">
+        <v>185</v>
+      </c>
+      <c r="J34">
+        <v>185</v>
+      </c>
+      <c r="L34">
+        <v>56</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="E35">
+        <v>665</v>
+      </c>
+      <c r="F35">
+        <v>0.75</v>
+      </c>
+      <c r="G35">
+        <v>1897.55</v>
+      </c>
+      <c r="H35">
+        <v>172</v>
+      </c>
+      <c r="J35">
+        <v>172</v>
+      </c>
+      <c r="L35">
+        <v>253</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="E36">
+        <v>773</v>
+      </c>
+      <c r="F36">
+        <v>0.66</v>
+      </c>
+      <c r="G36">
+        <v>1706.17</v>
+      </c>
+      <c r="H36">
+        <v>220</v>
+      </c>
+      <c r="J36">
+        <v>220</v>
+      </c>
+      <c r="L36">
+        <v>41</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B37">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="E37">
+        <v>891</v>
+      </c>
+      <c r="F37">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G37">
+        <v>1647.26</v>
+      </c>
+      <c r="H37">
+        <v>278</v>
+      </c>
+      <c r="J37">
+        <v>278</v>
+      </c>
+      <c r="L37">
+        <v>69</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B38">
+        <v>24</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="E38">
+        <v>924</v>
+      </c>
+      <c r="F38">
+        <v>0.52</v>
+      </c>
+      <c r="G38">
+        <v>1772.77</v>
+      </c>
+      <c r="H38">
+        <v>268</v>
+      </c>
+      <c r="J38">
+        <v>268</v>
+      </c>
+      <c r="L38">
+        <v>139</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7">
+        <v>211.9</v>
+      </c>
+      <c r="F40" s="7">
+        <v>2.38</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1957.55</v>
+      </c>
+      <c r="H40" s="7">
+        <v>37</v>
+      </c>
+      <c r="I40" s="7">
+        <v>38</v>
+      </c>
+      <c r="J40" s="7">
+        <v>67</v>
+      </c>
+      <c r="K40" s="7">
+        <v>106</v>
+      </c>
+      <c r="L40" s="7">
+        <v>174</v>
+      </c>
+      <c r="O40" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7">
+        <v>260.60000000000002</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1.93</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1722.72</v>
+      </c>
+      <c r="H41" s="7">
+        <v>63</v>
+      </c>
+      <c r="I41" s="7">
+        <v>61</v>
+      </c>
+      <c r="J41" s="7">
+        <v>108</v>
+      </c>
+      <c r="K41" s="7">
+        <v>181</v>
+      </c>
+      <c r="L41" s="7">
+        <v>49</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" s="7">
+        <v>3</v>
+      </c>
+      <c r="E42" s="7">
+        <v>288.89999999999998</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2036.8</v>
+      </c>
+      <c r="H42" s="7">
+        <v>67</v>
+      </c>
+      <c r="I42" s="7">
+        <v>64</v>
+      </c>
+      <c r="J42" s="7">
+        <v>143</v>
+      </c>
+      <c r="K42" s="7">
+        <v>76</v>
+      </c>
+      <c r="L42" s="7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" s="7">
+        <v>4</v>
+      </c>
+      <c r="E43" s="7">
+        <v>331.6</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1.52</v>
+      </c>
+      <c r="G43" s="7">
+        <v>1581.38</v>
+      </c>
+      <c r="H43" s="7">
+        <v>107</v>
+      </c>
+      <c r="I43" s="7">
+        <v>109</v>
+      </c>
+      <c r="J43" s="7">
+        <v>157</v>
+      </c>
+      <c r="K43" s="7">
+        <v>43</v>
+      </c>
+      <c r="L43" s="7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44" s="7">
+        <v>5</v>
+      </c>
+      <c r="E44" s="7">
+        <v>378.3</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1.34</v>
+      </c>
+      <c r="G44" s="7">
+        <v>1565.67</v>
+      </c>
+      <c r="H44" s="7">
+        <v>123</v>
+      </c>
+      <c r="I44" s="7">
+        <v>122</v>
+      </c>
+      <c r="J44" s="7">
+        <v>185</v>
+      </c>
+      <c r="K44" s="7">
+        <v>44</v>
+      </c>
+      <c r="L44" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>13</v>
+      </c>
+      <c r="C45" s="7">
+        <v>6</v>
+      </c>
+      <c r="E45" s="7">
+        <v>435.5</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G45" s="7">
+        <v>2021.11</v>
+      </c>
+      <c r="H45" s="7">
+        <v>197</v>
+      </c>
+      <c r="I45" s="7">
+        <v>202</v>
+      </c>
+      <c r="J45" s="7">
+        <v>156</v>
+      </c>
+      <c r="K45" s="7">
+        <v>75</v>
+      </c>
+      <c r="L45" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>14</v>
+      </c>
+      <c r="C46" s="7">
+        <v>7</v>
+      </c>
+      <c r="E46" s="7">
+        <v>520.4</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="G46" s="7">
+        <v>1628.5</v>
+      </c>
+      <c r="H46" s="7">
+        <v>195</v>
+      </c>
+      <c r="I46" s="7">
+        <v>188</v>
+      </c>
+      <c r="J46" s="7">
+        <v>108</v>
+      </c>
+      <c r="K46" s="7">
+        <v>46</v>
+      </c>
+      <c r="L46" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>16</v>
+      </c>
+      <c r="C47" s="7">
+        <v>8</v>
+      </c>
+      <c r="E47" s="7">
+        <v>585</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="G47" s="7">
+        <v>1539</v>
+      </c>
+      <c r="H47" s="7">
+        <v>184</v>
+      </c>
+      <c r="I47" s="7">
+        <v>184</v>
+      </c>
+      <c r="J47" s="7">
+        <v>92</v>
+      </c>
+      <c r="K47" s="7">
+        <v>45</v>
+      </c>
+      <c r="L47" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48">
+        <v>19</v>
+      </c>
+      <c r="C48" s="7">
+        <v>9</v>
+      </c>
+      <c r="E48" s="7">
+        <v>666.4</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="G48" s="7">
+        <v>1628.5</v>
+      </c>
+      <c r="H48" s="7">
+        <v>129</v>
+      </c>
+      <c r="I48" s="7">
+        <v>130</v>
+      </c>
+      <c r="J48" s="7">
+        <v>76</v>
+      </c>
+      <c r="K48" s="7">
+        <v>34</v>
+      </c>
+      <c r="L48" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49" s="7">
+        <v>10</v>
+      </c>
+      <c r="E49" s="7">
+        <v>773.9</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="G49" s="7">
+        <v>1442.15</v>
+      </c>
+      <c r="H49" s="7">
+        <v>183</v>
+      </c>
+      <c r="I49" s="7">
+        <v>188</v>
+      </c>
+      <c r="J49" s="7">
+        <v>127</v>
+      </c>
+      <c r="K49" s="7">
+        <v>69</v>
+      </c>
+      <c r="L49" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>23</v>
+      </c>
+      <c r="C50" s="7">
+        <v>11</v>
+      </c>
+      <c r="E50" s="7">
+        <v>891</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G50" s="7">
+        <v>1518.57</v>
+      </c>
+      <c r="H50" s="7">
+        <v>150</v>
+      </c>
+      <c r="I50" s="7">
+        <v>145</v>
+      </c>
+      <c r="J50" s="7">
+        <v>106</v>
+      </c>
+      <c r="K50" s="7">
+        <v>64</v>
+      </c>
+      <c r="L50" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="3">
+        <v>24</v>
+      </c>
+      <c r="C51" s="8">
+        <v>12</v>
+      </c>
+      <c r="E51" s="3">
+        <v>924.9</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1581.38</v>
+      </c>
+      <c r="H51" s="3">
+        <v>195</v>
+      </c>
+      <c r="I51" s="3">
+        <v>196</v>
+      </c>
+      <c r="J51" s="3">
+        <v>154</v>
+      </c>
+      <c r="K51" s="3">
+        <v>120</v>
+      </c>
+      <c r="L51" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="7">
+        <v>13</v>
+      </c>
+      <c r="E52">
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
+      <c r="G52" s="7">
+        <v>1957.55</v>
+      </c>
+      <c r="H52" s="7">
+        <v>20</v>
+      </c>
+      <c r="I52" s="7">
+        <v>19</v>
+      </c>
+      <c r="J52" s="7">
+        <v>91</v>
+      </c>
+      <c r="K52" s="7">
+        <v>157</v>
+      </c>
+      <c r="L52" s="7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" s="7">
+        <v>14</v>
+      </c>
+      <c r="G53" s="7">
+        <v>1722.72</v>
+      </c>
+      <c r="H53" s="7">
+        <v>24</v>
+      </c>
+      <c r="I53" s="7">
+        <v>24</v>
+      </c>
+      <c r="J53" s="7">
+        <v>135</v>
+      </c>
+      <c r="K53" s="7">
+        <v>239</v>
+      </c>
+      <c r="L53" s="7">
+        <v>46</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O53" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54" s="7">
+        <v>15</v>
+      </c>
+      <c r="G54" s="7">
+        <v>2036.8</v>
+      </c>
+      <c r="H54" s="7">
+        <v>24</v>
+      </c>
+      <c r="I54" s="7">
+        <v>22</v>
+      </c>
+      <c r="J54" s="7">
+        <v>164</v>
+      </c>
+      <c r="K54" s="7">
+        <v>45</v>
+      </c>
+      <c r="L54" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B55">
+        <v>8</v>
+      </c>
+      <c r="C55" s="7">
+        <v>16</v>
+      </c>
+      <c r="G55" s="7">
+        <v>1581.38</v>
+      </c>
+      <c r="H55" s="7">
+        <v>36</v>
+      </c>
+      <c r="I55" s="7">
+        <v>35</v>
+      </c>
+      <c r="J55" s="7">
+        <v>96</v>
+      </c>
+      <c r="K55" s="7">
+        <v>47</v>
+      </c>
+      <c r="L55" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56" s="7">
+        <v>17</v>
+      </c>
+      <c r="G56" s="7">
+        <v>1565.67</v>
+      </c>
+      <c r="H56" s="7">
+        <v>57</v>
+      </c>
+      <c r="I56" s="7">
+        <v>50</v>
+      </c>
+      <c r="J56" s="7">
+        <v>118</v>
+      </c>
+      <c r="K56" s="7">
+        <v>57</v>
+      </c>
+      <c r="L56" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B57">
+        <v>13</v>
+      </c>
+      <c r="C57" s="7">
+        <v>18</v>
+      </c>
+      <c r="G57" s="7">
+        <v>2021.11</v>
+      </c>
+      <c r="H57" s="7">
+        <v>52</v>
+      </c>
+      <c r="I57" s="7">
+        <v>56</v>
+      </c>
+      <c r="J57" s="7">
+        <v>86</v>
+      </c>
+      <c r="K57" s="7">
+        <v>75</v>
+      </c>
+      <c r="L57" s="7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B58">
+        <v>14</v>
+      </c>
+      <c r="C58" s="7">
+        <v>19</v>
+      </c>
+      <c r="G58" s="7">
+        <v>1628.5</v>
+      </c>
+      <c r="H58" s="7">
+        <v>47</v>
+      </c>
+      <c r="I58" s="7">
+        <v>68</v>
+      </c>
+      <c r="J58" s="7">
+        <v>98</v>
+      </c>
+      <c r="K58" s="7">
+        <v>67</v>
+      </c>
+      <c r="L58" s="7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B59">
+        <v>16</v>
+      </c>
+      <c r="C59" s="7">
+        <v>20</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1539</v>
+      </c>
+      <c r="H59" s="7">
+        <v>87</v>
+      </c>
+      <c r="I59" s="7">
+        <v>93</v>
+      </c>
+      <c r="J59" s="7">
+        <v>92</v>
+      </c>
+      <c r="K59" s="7">
+        <v>73</v>
+      </c>
+      <c r="L59" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B60">
+        <v>19</v>
+      </c>
+      <c r="C60" s="7">
+        <v>21</v>
+      </c>
+      <c r="G60" s="7">
+        <v>1628.5</v>
+      </c>
+      <c r="H60" s="7">
+        <v>45</v>
+      </c>
+      <c r="I60" s="7">
+        <v>45</v>
+      </c>
+      <c r="J60" s="7">
+        <v>66</v>
+      </c>
+      <c r="K60" s="7">
+        <v>65</v>
+      </c>
+      <c r="L60" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61" s="7">
+        <v>22</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1442.15</v>
+      </c>
+      <c r="H61" s="7">
+        <v>45</v>
+      </c>
+      <c r="I61" s="7">
+        <v>45</v>
+      </c>
+      <c r="J61" s="7">
+        <v>66</v>
+      </c>
+      <c r="K61" s="7">
+        <v>65</v>
+      </c>
+      <c r="L61" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B62">
+        <v>23</v>
+      </c>
+      <c r="C62" s="7">
+        <v>23</v>
+      </c>
+      <c r="G62" s="7">
+        <v>1518.57</v>
+      </c>
+      <c r="H62" s="7">
+        <v>114</v>
+      </c>
+      <c r="I62" s="7">
+        <v>101</v>
+      </c>
+      <c r="J62" s="7">
+        <v>123</v>
+      </c>
+      <c r="K62" s="7">
+        <v>95</v>
+      </c>
+      <c r="L62" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B63" s="3">
+        <v>24</v>
+      </c>
+      <c r="C63" s="8">
+        <v>24</v>
+      </c>
+      <c r="G63" s="3">
+        <v>1581.38</v>
+      </c>
+      <c r="H63" s="3">
+        <v>71</v>
+      </c>
+      <c r="I63" s="3">
+        <v>73</v>
+      </c>
+      <c r="J63" s="3">
+        <v>139</v>
+      </c>
+      <c r="K63" s="3">
+        <v>143</v>
+      </c>
+      <c r="L63" s="3">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -828,7 +2282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>